<commit_message>
new Fig S7 barplots showing individual replicates
</commit_message>
<xml_diff>
--- a/Ivanova source data.xlsx
+++ b/Ivanova source data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lcarey/Develop/Mendoza__ReplicationEvolution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC14CE3-9730-1F4B-BF67-70D8DF068882}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74892639-389F-B64C-90E5-7633F37CDA29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="0" windowWidth="25400" windowHeight="21600" firstSheet="12" activeTab="24" xr2:uid="{D2721514-58D2-3141-AF15-F76DE67DA8E9}"/>
+    <workbookView xWindow="2080" yWindow="0" windowWidth="25400" windowHeight="21600" firstSheet="12" activeTab="24" xr2:uid="{D2721514-58D2-3141-AF15-F76DE67DA8E9}"/>
   </bookViews>
   <sheets>
     <sheet name="fig1b" sheetId="1" r:id="rId1"/>
@@ -27918,7 +27918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC41F10-0D8F-F548-A8AD-84A94E2D8058}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -28275,10 +28277,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31956D2-5BDC-3A46-8B8B-6C5DE8CF5234}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A5" sqref="A5:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28341,276 +28343,276 @@
       </c>
       <c r="E4" s="24"/>
     </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7" t="s">
+        <v>244</v>
+      </c>
+      <c r="E7" t="s">
+        <v>245</v>
+      </c>
+      <c r="F7" t="s">
+        <v>246</v>
+      </c>
+      <c r="G7" t="s">
+        <v>247</v>
+      </c>
+      <c r="H7" t="s">
+        <v>248</v>
+      </c>
+      <c r="I7" t="s">
+        <v>249</v>
+      </c>
+      <c r="J7" t="s">
+        <v>250</v>
+      </c>
+      <c r="K7" t="s">
+        <v>251</v>
+      </c>
+      <c r="L7" t="s">
+        <v>252</v>
+      </c>
+      <c r="M7" t="s">
+        <v>253</v>
+      </c>
+    </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>259</v>
+      <c r="A8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8">
+        <v>77</v>
+      </c>
+      <c r="C8">
+        <v>81</v>
+      </c>
+      <c r="D8">
+        <v>79</v>
+      </c>
+      <c r="E8">
+        <v>45</v>
+      </c>
+      <c r="F8">
+        <v>47</v>
+      </c>
+      <c r="G8">
+        <v>42</v>
+      </c>
+      <c r="H8">
+        <v>40</v>
+      </c>
+      <c r="I8">
+        <v>43</v>
+      </c>
+      <c r="J8">
+        <v>41</v>
+      </c>
+      <c r="K8">
+        <v>39</v>
+      </c>
+      <c r="L8">
+        <v>40</v>
+      </c>
+      <c r="M8">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>242</v>
-      </c>
-      <c r="C9" t="s">
-        <v>243</v>
-      </c>
-      <c r="D9" t="s">
-        <v>244</v>
-      </c>
-      <c r="E9" t="s">
-        <v>245</v>
-      </c>
-      <c r="F9" t="s">
-        <v>246</v>
-      </c>
-      <c r="G9" t="s">
-        <v>247</v>
-      </c>
-      <c r="H9" t="s">
-        <v>248</v>
-      </c>
-      <c r="I9" t="s">
-        <v>249</v>
-      </c>
-      <c r="J9" t="s">
-        <v>250</v>
-      </c>
-      <c r="K9" t="s">
-        <v>251</v>
-      </c>
-      <c r="L9" t="s">
-        <v>252</v>
-      </c>
-      <c r="M9" t="s">
-        <v>253</v>
+      <c r="A9" t="s">
+        <v>261</v>
+      </c>
+      <c r="B9">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <v>24</v>
+      </c>
+      <c r="E9">
+        <v>62</v>
+      </c>
+      <c r="F9">
+        <v>60</v>
+      </c>
+      <c r="G9">
+        <v>60</v>
+      </c>
+      <c r="H9">
+        <v>60</v>
+      </c>
+      <c r="I9">
+        <v>57</v>
+      </c>
+      <c r="J9">
+        <v>67</v>
+      </c>
+      <c r="K9">
+        <v>61</v>
+      </c>
+      <c r="L9">
+        <v>62</v>
+      </c>
+      <c r="M9">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>260</v>
+        <v>106</v>
       </c>
       <c r="B10">
-        <v>77</v>
+        <f>SUM(B8:B9)</f>
+        <v>100</v>
       </c>
       <c r="C10">
-        <v>81</v>
+        <f t="shared" ref="C10:M10" si="0">SUM(C8:C9)</f>
+        <v>109</v>
       </c>
       <c r="D10">
-        <v>79</v>
+        <f t="shared" si="0"/>
+        <v>103</v>
       </c>
       <c r="E10">
-        <v>45</v>
+        <f t="shared" si="0"/>
+        <v>107</v>
       </c>
       <c r="F10">
-        <v>47</v>
+        <f t="shared" si="0"/>
+        <v>107</v>
       </c>
       <c r="G10">
-        <v>42</v>
+        <f t="shared" si="0"/>
+        <v>102</v>
       </c>
       <c r="H10">
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="I10">
-        <v>43</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="J10">
-        <v>41</v>
+        <f t="shared" si="0"/>
+        <v>108</v>
       </c>
       <c r="K10">
-        <v>39</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="L10">
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>102</v>
       </c>
       <c r="M10">
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B11">
-        <v>23</v>
+        <f>(B8/B10)*100</f>
+        <v>77</v>
       </c>
       <c r="C11">
-        <v>28</v>
+        <f t="shared" ref="C11:M11" si="1">(C8/C10)*100</f>
+        <v>74.311926605504581</v>
       </c>
       <c r="D11">
-        <v>24</v>
+        <f t="shared" si="1"/>
+        <v>76.699029126213588</v>
       </c>
       <c r="E11">
-        <v>62</v>
+        <f t="shared" si="1"/>
+        <v>42.056074766355138</v>
       </c>
       <c r="F11">
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>43.925233644859816</v>
       </c>
       <c r="G11">
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>41.17647058823529</v>
       </c>
       <c r="H11">
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
       <c r="I11">
-        <v>57</v>
+        <f t="shared" si="1"/>
+        <v>43</v>
       </c>
       <c r="J11">
-        <v>67</v>
+        <f t="shared" si="1"/>
+        <v>37.962962962962962</v>
       </c>
       <c r="K11">
-        <v>61</v>
+        <f t="shared" si="1"/>
+        <v>39</v>
       </c>
       <c r="L11">
-        <v>62</v>
+        <f t="shared" si="1"/>
+        <v>39.215686274509807</v>
       </c>
       <c r="M11">
-        <v>38</v>
+        <f t="shared" si="1"/>
+        <v>29.629629629629626</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B12">
-        <f>SUM(B10:B11)</f>
-        <v>100</v>
+        <v>263</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:M12" si="0">SUM(C10:C11)</f>
-        <v>109</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>103</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>107</v>
+        <f>AVERAGE(B11:D11)</f>
+        <v>76.003651910572728</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
-        <v>107</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>102</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>AVERAGE(E11:G11)</f>
+        <v>42.385926333150081</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>AVERAGE(H11:J11)</f>
+        <v>40.320987654320987</v>
       </c>
       <c r="L12">
-        <f t="shared" si="0"/>
-        <v>102</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="0"/>
-        <v>54</v>
+        <f>AVERAGE(K11:M11)</f>
+        <v>35.948438634713142</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>262</v>
-      </c>
-      <c r="B13">
-        <f>(B10/B12)*100</f>
-        <v>77</v>
+        <v>264</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:M13" si="1">(C10/C12)*100</f>
-        <v>74.311926605504581</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="1"/>
-        <v>76.699029126213588</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>42.056074766355138</v>
+        <f>STDEV(B11:D11)/SQRT(3)</f>
+        <v>0.85031303011946968</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
-        <v>43.925233644859816</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="1"/>
-        <v>41.17647058823529</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f>STDEV(E11:G11)/SQRT(3)</f>
+        <v>0.8104579214768568</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="1"/>
-        <v>37.962962962962962</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="1"/>
-        <v>39</v>
+        <f>STDEV(H11:J11)/SQRT(3)</f>
+        <v>1.4628978471730443</v>
       </c>
       <c r="L13">
-        <f t="shared" si="1"/>
-        <v>39.215686274509807</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="1"/>
-        <v>29.629629629629626</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>263</v>
-      </c>
-      <c r="C14">
-        <f>AVERAGE(B13:D13)</f>
-        <v>76.003651910572728</v>
-      </c>
-      <c r="F14">
-        <f>AVERAGE(E13:G13)</f>
-        <v>42.385926333150081</v>
-      </c>
-      <c r="I14">
-        <f>AVERAGE(H13:J13)</f>
-        <v>40.320987654320987</v>
-      </c>
-      <c r="L14">
-        <f>AVERAGE(K13:M13)</f>
-        <v>35.948438634713142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>264</v>
-      </c>
-      <c r="C15">
-        <f>STDEV(B13:D13)/SQRT(3)</f>
-        <v>0.85031303011946968</v>
-      </c>
-      <c r="F15">
-        <f>STDEV(E13:G13)/SQRT(3)</f>
-        <v>0.8104579214768568</v>
-      </c>
-      <c r="I15">
-        <f>STDEV(H13:J13)/SQRT(3)</f>
-        <v>1.4628978471730443</v>
-      </c>
-      <c r="L15">
-        <f>STDEV(K13:M13)/SQRT(3)</f>
+        <f>STDEV(K11:M11)/SQRT(3)</f>
         <v>3.1600179627283005</v>
       </c>
     </row>

</xml_diff>